<commit_message>
MSD Results of Force
expected MSD need to be fixed
</commit_message>
<xml_diff>
--- a/MSD Results/msd_100.xlsx
+++ b/MSD Results/msd_100.xlsx
@@ -427,7 +427,7 @@
         <v>0.009674836071919213</v>
       </c>
       <c r="C4">
-        <v>0.009764374442686428</v>
+        <v>0.00878560919904809</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -438,7 +438,7 @@
         <v>0.02141595285011544</v>
       </c>
       <c r="C5">
-        <v>0.0215492283826515</v>
+        <v>0.01763990336000434</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -449,7 +449,7 @@
         <v>0.03746150615596378</v>
       </c>
       <c r="C6">
-        <v>0.03761296481598453</v>
+        <v>0.02791388803469015</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -460,7 +460,7 @@
         <v>0.05760156614280998</v>
       </c>
       <c r="C7">
-        <v>0.05773700090037102</v>
+        <v>0.03914597648032975</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -471,7 +471,7 @@
         <v>0.08163644136343606</v>
       </c>
       <c r="C8">
-        <v>0.08178270660511414</v>
+        <v>0.05010911626940852</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -482,7 +482,7 @@
         <v>0.1093761794374268</v>
       </c>
       <c r="C9">
-        <v>0.1094644863121297</v>
+        <v>0.06076618351247165</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -493,7 +493,7 @@
         <v>0.1406400920712789</v>
       </c>
       <c r="C10">
-        <v>0.1406859561980342</v>
+        <v>0.071615180289929</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -504,7 +504,7 @@
         <v>0.1752563032435468</v>
       </c>
       <c r="C11">
-        <v>0.1753187707847842</v>
+        <v>0.0820871954407735</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -515,7 +515,7 @@
         <v>0.2130613194252668</v>
       </c>
       <c r="C12">
-        <v>0.212988577504957</v>
+        <v>0.09106758365539509</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -526,7 +526,7 @@
         <v>0.2538996207609734</v>
       </c>
       <c r="C13">
-        <v>0.2534114961788754</v>
+        <v>0.0986590525065361</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -537,7 +537,7 @@
         <v>0.2976232721880532</v>
       </c>
       <c r="C14">
-        <v>0.2967179095413726</v>
+        <v>0.1057811423396419</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -548,7 +548,7 @@
         <v>0.3440915535220324</v>
       </c>
       <c r="C15">
-        <v>0.3428153502364119</v>
+        <v>0.1119530566309999</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -559,7 +559,7 @@
         <v>0.3931706075828192</v>
       </c>
       <c r="C16">
-        <v>0.3914905816772996</v>
+        <v>0.1178187723758293</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -570,7 +570,7 @@
         <v>0.4447331054820296</v>
       </c>
       <c r="C17">
-        <v>0.4420685954796356</v>
+        <v>0.1236921727347812</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -581,7 +581,7 @@
         <v>0.4986579282344432</v>
       </c>
       <c r="C18">
-        <v>0.4948596030823904</v>
+        <v>0.1281477435339107</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -592,7 +592,7 @@
         <v>0.5548298638974534</v>
       </c>
       <c r="C19">
-        <v>0.5490863389153169</v>
+        <v>0.1333107848195079</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -603,7 +603,7 @@
         <v>0.6131393194811983</v>
       </c>
       <c r="C20">
-        <v>0.6049344827298195</v>
+        <v>0.1382922553624908</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -614,7 +614,7 @@
         <v>0.6734820469090024</v>
       </c>
       <c r="C21">
-        <v>0.6636864267642368</v>
+        <v>0.1422176305282399</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -625,7 +625,7 @@
         <v>0.7357588823428847</v>
       </c>
       <c r="C22">
-        <v>0.7242109924414881</v>
+        <v>0.1458894937587656</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -636,7 +636,7 @@
         <v>0.7998754982223106</v>
       </c>
       <c r="C23">
-        <v>0.7871142732790487</v>
+        <v>0.1485582428590578</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -647,7 +647,7 @@
         <v>0.8657421673961592</v>
       </c>
       <c r="C24">
-        <v>0.8516437300009922</v>
+        <v>0.1505592490687245</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -658,7 +658,7 @@
         <v>0.9332735387581064</v>
       </c>
       <c r="C25">
-        <v>0.9177995316873249</v>
+        <v>0.1525012081302259</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -669,7 +669,7 @@
         <v>1.002388423824404</v>
       </c>
       <c r="C26">
-        <v>0.9857037642009377</v>
+        <v>0.1542242940635086</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -680,7 +680,7 @@
         <v>1.07300959372038</v>
       </c>
       <c r="C27">
-        <v>1.055869921134455</v>
+        <v>0.1555185563646166</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -691,7 +691,7 @@
         <v>1.145063586068025</v>
       </c>
       <c r="C28">
-        <v>1.128359177062147</v>
+        <v>0.155921483470101</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -702,7 +702,7 @@
         <v>1.218480521291783</v>
       </c>
       <c r="C29">
-        <v>1.20330106591217</v>
+        <v>0.1573983540029121</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -713,7 +713,7 @@
         <v>1.293193927883213</v>
       </c>
       <c r="C30">
-        <v>1.279503589659629</v>
+        <v>0.158779307678483</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -724,7 +724,7 @@
         <v>1.369140576187596</v>
       </c>
       <c r="C31">
-        <v>1.357266829006439</v>
+        <v>0.1599222849955843</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -735,7 +735,7 @@
         <v>1.44626032029686</v>
       </c>
       <c r="C32">
-        <v>1.435226969107084</v>
+        <v>0.1599274277281699</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -746,7 +746,7 @@
         <v>1.524495947653486</v>
       </c>
       <c r="C33">
-        <v>1.51341489902897</v>
+        <v>0.1600218246873647</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -757,7 +757,7 @@
         <v>1.603793035989311</v>
       </c>
       <c r="C34">
-        <v>1.592650155375509</v>
+        <v>0.1601733270423134</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -768,7 +768,7 @@
         <v>1.684099817241508</v>
       </c>
       <c r="C35">
-        <v>1.67199267705986</v>
+        <v>0.1607265025551962</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -779,7 +779,7 @@
         <v>1.76536704810547</v>
       </c>
       <c r="C36">
-        <v>1.751418249830069</v>
+        <v>0.1611602632836112</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -790,7 +790,7 @@
         <v>1.84754788690089</v>
       </c>
       <c r="C37">
-        <v>1.830693195452586</v>
+        <v>0.1614729027821417</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -801,7 +801,7 @@
         <v>1.930597776443173</v>
       </c>
       <c r="C38">
-        <v>1.911332719507737</v>
+        <v>0.1615301439829503</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -812,7 +812,7 @@
         <v>2.014474332627255</v>
       </c>
       <c r="C39">
-        <v>1.994242713970876</v>
+        <v>0.1618006541914286</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -823,7 +823,7 @@
         <v>2.09913723844527</v>
       </c>
       <c r="C40">
-        <v>2.079264432079217</v>
+        <v>0.1620359341226862</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -834,7 +834,7 @@
         <v>2.184548143173028</v>
       </c>
       <c r="C41">
-        <v>2.166764378760166</v>
+        <v>0.162302284171273</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -845,7 +845,7 @@
         <v>2.270670566473226</v>
       </c>
       <c r="C42">
-        <v>2.254397963990263</v>
+        <v>0.1630063578898919</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -856,7 +856,7 @@
         <v>2.357469807175609</v>
       </c>
       <c r="C43">
-        <v>2.341194064631165</v>
+        <v>0.163310457943063</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -867,7 +867,7 @@
         <v>2.444912856505964</v>
       </c>
       <c r="C44">
-        <v>2.430198913422585</v>
+        <v>0.1624716488005847</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -878,7 +878,7 @@
         <v>2.532968315546993</v>
       </c>
       <c r="C45">
-        <v>2.519769856747016</v>
+        <v>0.1613114468399834</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -889,7 +889,7 @@
         <v>2.621606316724668</v>
       </c>
       <c r="C46">
-        <v>2.611668148211874</v>
+        <v>0.1609078022982006</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -900,7 +900,7 @@
         <v>2.710798449123729</v>
       </c>
       <c r="C47">
-        <v>2.704219220851991</v>
+        <v>0.1611072242900752</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -911,7 +911,7 @@
         <v>2.800517687445608</v>
       </c>
       <c r="C48">
-        <v>2.79818949798583</v>
+        <v>0.1618616622760173</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -922,7 +922,7 @@
         <v>2.8907383244311</v>
       </c>
       <c r="C49">
-        <v>2.892693961422349</v>
+        <v>0.162973963921389</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -933,7 +933,7 @@
         <v>2.981435906578826</v>
       </c>
       <c r="C50">
-        <v>2.986632815067804</v>
+        <v>0.1630015042296124</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -944,7 +944,7 @@
         <v>3.072587172998741</v>
       </c>
       <c r="C51">
-        <v>3.080065514295103</v>
+        <v>0.1634984561009809</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -955,7 +955,7 @@
         <v>3.164169997247797</v>
       </c>
       <c r="C52">
-        <v>3.175545099112409</v>
+        <v>0.1644432849314499</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -966,7 +966,7 @@
         <v>3.256163332002306</v>
       </c>
       <c r="C53">
-        <v>3.270599850590896</v>
+        <v>0.1653742741076255</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -977,7 +977,7 @@
         <v>3.348547156428668</v>
       </c>
       <c r="C54">
-        <v>3.366108204075895</v>
+        <v>0.1663454877172831</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -988,7 +988,7 @@
         <v>3.44130242612086</v>
       </c>
       <c r="C55">
-        <v>3.460116918975426</v>
+        <v>0.1666480547421834</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -999,7 +999,7 @@
         <v>3.5344110254795</v>
       </c>
       <c r="C56">
-        <v>3.553632632114085</v>
+        <v>0.1676541239468862</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1010,7 +1010,7 @@
         <v>3.627855722413415</v>
       </c>
       <c r="C57">
-        <v>3.647717142297222</v>
+        <v>0.1685477997214688</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1021,7 +1021,7 @@
         <v>3.721620125250436</v>
       </c>
       <c r="C58">
-        <v>3.742586537011237</v>
+        <v>0.1677809994680456</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1032,7 +1032,7 @@
         <v>3.815688641749677</v>
       </c>
       <c r="C59">
-        <v>3.836533035463772</v>
+        <v>0.1663852842208756</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1043,7 +1043,7 @@
         <v>3.910046440112815</v>
       </c>
       <c r="C60">
-        <v>3.930184904084003</v>
+        <v>0.165777599087067</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1054,7 +1054,7 @@
         <v>4.004679411896865</v>
       </c>
       <c r="C61">
-        <v>4.02197043023696</v>
+        <v>0.1652140221772581</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1065,7 +1065,7 @@
         <v>4.099574136735728</v>
       </c>
       <c r="C62">
-        <v>4.112833107507608</v>
+        <v>0.1646920749254976</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1076,7 +1076,7 @@
         <v>4.194717848782282</v>
       </c>
       <c r="C63">
-        <v>4.2052633213952</v>
+        <v>0.164555703992487</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1087,7 +1087,7 @@
         <v>4.290098404787115</v>
       </c>
       <c r="C64">
-        <v>4.296757519303133</v>
+        <v>0.1647962160861574</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1098,7 +1098,7 @@
         <v>4.385704253734081</v>
       </c>
       <c r="C65">
-        <v>4.389203681080273</v>
+        <v>0.1665869645835208</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1109,7 +1109,7 @@
         <v>4.481524407956733</v>
       </c>
       <c r="C66">
-        <v>4.48486654117352</v>
+        <v>0.1676914817999143</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1120,7 +1120,7 @@
         <v>4.577548415663444</v>
       </c>
       <c r="C67">
-        <v>4.580123777459661</v>
+        <v>0.1679341544472869</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1131,7 +1131,7 @@
         <v>4.67376633480248</v>
       </c>
       <c r="C68">
-        <v>4.673995342140144</v>
+        <v>0.1682905011774078</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1142,7 +1142,7 @@
         <v>4.77016870820169</v>
       </c>
       <c r="C69">
-        <v>4.76797222381064</v>
+        <v>0.1690402441355317</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1153,7 +1153,7 @@
         <v>4.866746539920653</v>
       </c>
       <c r="C70">
-        <v>4.863435495291911</v>
+        <v>0.16908651470713</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1164,7 +1164,7 @@
         <v>4.963491272756136</v>
       </c>
       <c r="C71">
-        <v>4.957446998185795</v>
+        <v>0.1696385785747392</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1175,7 +1175,7 @@
         <v>5.060394766844637</v>
       </c>
       <c r="C72">
-        <v>5.053845502747697</v>
+        <v>0.1698172400467191</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1186,7 +1186,7 @@
         <v>5.157449279308479</v>
       </c>
       <c r="C73">
-        <v>5.149007373552093</v>
+        <v>0.1704760504174024</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1197,7 +1197,7 @@
         <v>5.254647444894585</v>
       </c>
       <c r="C74">
-        <v>5.243558599021839</v>
+        <v>0.1696908501681237</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1208,7 +1208,7 @@
         <v>5.351982257557512</v>
       </c>
       <c r="C75">
-        <v>5.338717049217992</v>
+        <v>0.1696668972329304</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1219,7 +1219,7 @@
         <v>5.44944705294068</v>
       </c>
       <c r="C76">
-        <v>5.432016943534971</v>
+        <v>0.1706198939246768</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1230,7 +1230,7 @@
         <v>5.547035491712018</v>
       </c>
       <c r="C77">
-        <v>5.524013950539717</v>
+        <v>0.1703866375464358</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1241,7 +1241,7 @@
         <v>5.644741543712332</v>
       </c>
       <c r="C78">
-        <v>5.61931254570487</v>
+        <v>0.1698034063473605</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1252,7 +1252,7 @@
         <v>5.742559472876755</v>
       </c>
       <c r="C79">
-        <v>5.715461009928634</v>
+        <v>0.169190359772805</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1263,7 +1263,7 @@
         <v>5.84048382289161</v>
       </c>
       <c r="C80">
-        <v>5.814042945691527</v>
+        <v>0.1693450927372112</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1274,7 +1274,7 @@
         <v>5.938509403550774</v>
       </c>
       <c r="C81">
-        <v>5.914315345372083</v>
+        <v>0.1681581410998196</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1285,7 +1285,7 @@
         <v>6.036631277777468</v>
       </c>
       <c r="C82">
-        <v>6.018145795804263</v>
+        <v>0.1671321992309346</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1296,7 +1296,7 @@
         <v>6.134844749278987</v>
       </c>
       <c r="C83">
-        <v>6.120620336310553</v>
+        <v>0.1665675091425781</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1307,7 +1307,7 @@
         <v>6.233145350803523</v>
       </c>
       <c r="C84">
-        <v>6.222090758651102</v>
+        <v>0.1660458426844484</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1318,7 +1318,7 @@
         <v>6.33152883296971</v>
       </c>
       <c r="C85">
-        <v>6.323486587526951</v>
+        <v>0.1653716231067811</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1329,7 +1329,7 @@
         <v>6.429991153640955</v>
       </c>
       <c r="C86">
-        <v>6.427355564744395</v>
+        <v>0.1642888211480173</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1340,7 +1340,7 @@
         <v>6.528528467817999</v>
       </c>
       <c r="C87">
-        <v>6.527899799666858</v>
+        <v>0.1629424383221244</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1351,7 +1351,7 @@
         <v>6.627137118024402</v>
       </c>
       <c r="C88">
-        <v>6.628254548318795</v>
+        <v>0.1624974540295661</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1362,7 +1362,7 @@
         <v>6.72581362516096</v>
       </c>
       <c r="C89">
-        <v>6.727055105585507</v>
+        <v>0.1628825334539284</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1373,7 +1373,7 @@
         <v>6.824554679806138</v>
       </c>
       <c r="C90">
-        <v>6.824272393288985</v>
+        <v>0.1627618535610183</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1384,7 +1384,7 @@
         <v>6.923357133940792</v>
       </c>
       <c r="C91">
-        <v>6.92376678183673</v>
+        <v>0.1624840865646699</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1395,7 +1395,7 @@
         <v>7.022217993076485</v>
       </c>
       <c r="C92">
-        <v>7.025582900317208</v>
+        <v>0.1619844455513476</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1406,7 +1406,7 @@
         <v>7.121134408767706</v>
       </c>
       <c r="C93">
-        <v>7.125573453877672</v>
+        <v>0.16154402070179</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1417,7 +1417,7 @@
         <v>7.220103671489268</v>
       </c>
       <c r="C94">
-        <v>7.227155189626295</v>
+        <v>0.1613777058135605</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1428,7 +1428,7 @@
         <v>7.319123203861087</v>
       </c>
       <c r="C95">
-        <v>7.32755873211287</v>
+        <v>0.1615363367619487</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1439,7 +1439,7 @@
         <v>7.418190554203392</v>
       </c>
       <c r="C96">
-        <v>7.430395869057336</v>
+        <v>0.1620283128353682</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1450,7 +1450,7 @@
         <v>7.517303390406241</v>
       </c>
       <c r="C97">
-        <v>7.534213318347108</v>
+        <v>0.1633429868081563</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1461,7 +1461,7 @@
         <v>7.616459494098041</v>
       </c>
       <c r="C98">
-        <v>7.633891107524033</v>
+        <v>0.1642615532157029</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1472,7 +1472,7 @@
         <v>7.715656755098452</v>
       </c>
       <c r="C99">
-        <v>7.729923188144431</v>
+        <v>0.1649684492874969</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1483,7 +1483,7 @@
         <v>7.81489316614185</v>
       </c>
       <c r="C100">
-        <v>7.825320777596429</v>
+        <v>0.1658473256627086</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1494,7 +1494,7 @@
         <v>7.914166817858105</v>
       </c>
       <c r="C101">
-        <v>7.918405149317591</v>
+        <v>0.1675755104094715</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1505,7 +1505,7 @@
         <v>8.013475893998171</v>
       </c>
       <c r="C102">
-        <v>8.01249679402947</v>
+        <v>0.1689456357408397</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1516,7 +1516,7 @@
         <v>8.112818666892514</v>
       </c>
       <c r="C103">
-        <v>8.110226975047501</v>
+        <v>0.1699169572773373</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1527,7 +1527,7 @@
         <v>8.212193493131032</v>
       </c>
       <c r="C104">
-        <v>8.205100319451169</v>
+        <v>0.171628304191309</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1538,7 +1538,7 @@
         <v>8.311598809453685</v>
       </c>
       <c r="C105">
-        <v>8.300261036435611</v>
+        <v>0.1729107192635843</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1549,7 +1549,7 @@
         <v>8.411033128841522</v>
       </c>
       <c r="C106">
-        <v>8.394670131443515</v>
+        <v>0.1734635673376794</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1560,7 +1560,7 @@
         <v>8.510495036798362</v>
       </c>
       <c r="C107">
-        <v>8.489745471068236</v>
+        <v>0.1728819441210485</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1571,7 +1571,7 @@
         <v>8.609983187813821</v>
       </c>
       <c r="C108">
-        <v>8.585526905221245</v>
+        <v>0.1737842765429697</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1582,7 +1582,7 @@
         <v>8.709496301998824</v>
       </c>
       <c r="C109">
-        <v>8.681753276075268</v>
+        <v>0.1737732309400402</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1593,7 +1593,7 @@
         <v>8.809033161885226</v>
       </c>
       <c r="C110">
-        <v>8.777695175831116</v>
+        <v>0.1738773173084446</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1604,7 +1604,7 @@
         <v>8.908592609381506</v>
       </c>
       <c r="C111">
-        <v>8.873498382942341</v>
+        <v>0.17281664141478</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1615,7 +1615,7 @@
         <v>9.008173542876929</v>
       </c>
       <c r="C112">
-        <v>8.970729035630301</v>
+        <v>0.1720017309150978</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1626,7 +1626,7 @@
         <v>9.107774914486953</v>
       </c>
       <c r="C113">
-        <v>9.068170159498472</v>
+        <v>0.1714958195809201</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1637,7 +1637,7 @@
         <v>9.207395727432967</v>
       </c>
       <c r="C114">
-        <v>9.162333879299316</v>
+        <v>0.1705618194659395</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1648,7 +1648,7 @@
         <v>9.307035033549825</v>
       </c>
       <c r="C115">
-        <v>9.256380699398218</v>
+        <v>0.1700583890893725</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1659,7 +1659,7 @@
         <v>9.406691930914944</v>
       </c>
       <c r="C116">
-        <v>9.350182972244877</v>
+        <v>0.1697392008452818</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1670,7 +1670,7 @@
         <v>9.50636556159302</v>
       </c>
       <c r="C117">
-        <v>9.439450882449425</v>
+        <v>0.1696720709837865</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1681,7 +1681,7 @@
         <v>9.606055109490754</v>
       </c>
       <c r="C118">
-        <v>9.528439170446099</v>
+        <v>0.1702594047358094</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1692,7 +1692,7 @@
         <v>9.705759798316178</v>
       </c>
       <c r="C119">
-        <v>9.616736907033886</v>
+        <v>0.1710383245320914</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1703,7 +1703,7 @@
         <v>9.805478889637538</v>
       </c>
       <c r="C120">
-        <v>9.703389944417101</v>
+        <v>0.1712477261652448</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1714,7 +1714,7 @@
         <v>9.905211681036818</v>
       </c>
       <c r="C121">
-        <v>9.786689510218453</v>
+        <v>0.1717403790781827</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1725,7 +1725,7 @@
         <v>10.00495750435333</v>
       </c>
       <c r="C122">
-        <v>9.870114452831642</v>
+        <v>0.1721569189624212</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1736,7 +1736,7 @@
         <v>10.10471572401298</v>
       </c>
       <c r="C123">
-        <v>9.955344501095437</v>
+        <v>0.1735784457907764</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1747,7 +1747,7 @@
         <v>10.20448573543897</v>
       </c>
       <c r="C124">
-        <v>10.04429073305594</v>
+        <v>0.174759723545598</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1758,7 +1758,7 @@
         <v>10.30426696354008</v>
       </c>
       <c r="C125">
-        <v>10.13470156884441</v>
+        <v>0.1751223365837041</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1769,7 +1769,7 @@
         <v>10.40405886127259</v>
       </c>
       <c r="C126">
-        <v>10.22575495660536</v>
+        <v>0.1745239854603901</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1780,7 +1780,7 @@
         <v>10.50386090827246</v>
       </c>
       <c r="C127">
-        <v>10.31683965876509</v>
+        <v>0.1755384168850248</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1791,7 +1791,7 @@
         <v>10.60367260955406</v>
       </c>
       <c r="C128">
-        <v>10.40820073930347</v>
+        <v>0.1751195161012311</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1802,7 +1802,7 @@
         <v>10.70349349427252</v>
       </c>
       <c r="C129">
-        <v>10.49982680659913</v>
+        <v>0.1738834526460733</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1813,7 +1813,7 @@
         <v>10.80332311454635</v>
       </c>
       <c r="C130">
-        <v>10.58957142194707</v>
+        <v>0.1737641455347428</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1824,7 +1824,7 @@
         <v>10.90316104433747</v>
       </c>
       <c r="C131">
-        <v>10.68222048771384</v>
+        <v>0.1739020499230994</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1835,7 +1835,7 @@
         <v>11.00300687838596</v>
       </c>
       <c r="C132">
-        <v>10.77448736695018</v>
+        <v>0.1732010817179874</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1846,7 +1846,7 @@
         <v>11.10286023119662</v>
       </c>
       <c r="C133">
-        <v>10.86667756935048</v>
+        <v>0.1714797574126983</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1857,7 +1857,7 @@
         <v>11.2027207360751</v>
       </c>
       <c r="C134">
-        <v>10.96096399540543</v>
+        <v>0.1693816028620835</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1868,7 +1868,7 @@
         <v>11.30258804421093</v>
       </c>
       <c r="C135">
-        <v>11.05696232348877</v>
+        <v>0.1683458600680302</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1879,7 +1879,7 @@
         <v>11.40246182380535</v>
       </c>
       <c r="C136">
-        <v>11.15067234900832</v>
+        <v>0.1661536838636007</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1890,7 +1890,7 @@
         <v>11.50234175924158</v>
       </c>
       <c r="C137">
-        <v>11.24072941851295</v>
+        <v>0.1637704497866593</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1901,7 +1901,7 @@
         <v>11.60222755029569</v>
       </c>
       <c r="C138">
-        <v>11.32960941425461</v>
+        <v>0.1612928657852298</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -1912,7 +1912,7 @@
         <v>11.70211891138582</v>
       </c>
       <c r="C139">
-        <v>11.41639596827327</v>
+        <v>0.1590899766189891</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -1923,7 +1923,7 @@
         <v>11.8020155708581</v>
       </c>
       <c r="C140">
-        <v>11.50288699501825</v>
+        <v>0.1567818757748944</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1934,7 +1934,7 @@
         <v>11.90191727030739</v>
       </c>
       <c r="C141">
-        <v>11.5911435267622</v>
+        <v>0.1546975798138235</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -1945,7 +1945,7 @@
         <v>12.00182376393111</v>
       </c>
       <c r="C142">
-        <v>11.67853037520477</v>
+        <v>0.1551161585669093</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -1956,7 +1956,7 @@
         <v>12.10173481791461</v>
       </c>
       <c r="C143">
-        <v>11.76647270652681</v>
+        <v>0.1567008134157369</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -1967,7 +1967,7 @@
         <v>12.20165020984653</v>
       </c>
       <c r="C144">
-        <v>11.85126699025768</v>
+        <v>0.1579123304354674</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -1978,7 +1978,7 @@
         <v>12.30156972816262</v>
       </c>
       <c r="C145">
-        <v>11.93437815069134</v>
+        <v>0.1594794679810595</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -1989,7 +1989,7 @@
         <v>12.40149317161675</v>
       </c>
       <c r="C146">
-        <v>12.01844313926533</v>
+        <v>0.1610479497590116</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2000,7 +2000,7 @@
         <v>12.50142034877769</v>
       </c>
       <c r="C147">
-        <v>12.10305977349151</v>
+        <v>0.1618954581011907</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2011,7 +2011,7 @@
         <v>12.60135107755039</v>
       </c>
       <c r="C148">
-        <v>12.1928493232805</v>
+        <v>0.1629927257760558</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2022,7 +2022,7 @@
         <v>12.70128518472071</v>
       </c>
       <c r="C149">
-        <v>12.27660467083073</v>
+        <v>0.1641122674927038</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2033,7 +2033,7 @@
         <v>12.80122250552226</v>
       </c>
       <c r="C150">
-        <v>12.35940821590697</v>
+        <v>0.1656351828887222</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2044,7 +2044,7 @@
         <v>12.90116288322439</v>
       </c>
       <c r="C151">
-        <v>12.44366174676249</v>
+        <v>0.1668634589941126</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2055,7 +2055,7 @@
         <v>13.0011061687403</v>
       </c>
       <c r="C152">
-        <v>12.53125258877511</v>
+        <v>0.1669937088572863</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2066,7 +2066,7 @@
         <v>13.10105222025423</v>
       </c>
       <c r="C153">
-        <v>12.6182154565193</v>
+        <v>0.1674028994815472</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2077,7 +2077,7 @@
         <v>13.20100090286688</v>
       </c>
       <c r="C154">
-        <v>12.71230191683757</v>
+        <v>0.1683111138017523</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2088,7 +2088,7 @@
         <v>13.30095208825804</v>
       </c>
       <c r="C155">
-        <v>12.80803801252769</v>
+        <v>0.1693474728699976</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2099,7 +2099,7 @@
         <v>13.40090565436577</v>
       </c>
       <c r="C156">
-        <v>12.90507703485914</v>
+        <v>0.1708265759798278</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2110,7 +2110,7 @@
         <v>13.50086148508115</v>
       </c>
       <c r="C157">
-        <v>13.00402348638781</v>
+        <v>0.1719210879253189</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2121,7 +2121,7 @@
         <v>13.60081946995796</v>
       </c>
       <c r="C158">
-        <v>13.10211873547402</v>
+        <v>0.1720996244982718</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2132,7 +2132,7 @@
         <v>13.70077950393651</v>
       </c>
       <c r="C159">
-        <v>13.20075154369818</v>
+        <v>0.1723601403995868</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2143,7 +2143,7 @@
         <v>13.80074148708092</v>
       </c>
       <c r="C160">
-        <v>13.30119201877389</v>
+        <v>0.1727006538384711</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2154,7 +2154,7 @@
         <v>13.90070532432926</v>
       </c>
       <c r="C161">
-        <v>13.4026714564419</v>
+        <v>0.1730908959522516</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2165,7 +2165,7 @@
         <v>14.0006709252558</v>
       </c>
       <c r="C162">
-        <v>13.50034744731851</v>
+        <v>0.1732721701773018</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2176,7 +2176,7 @@
         <v>14.10063820384496</v>
       </c>
       <c r="C163">
-        <v>13.59529737924841</v>
+        <v>0.1736320808039539</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2187,7 +2187,7 @@
         <v>14.20060707827616</v>
       </c>
       <c r="C164">
-        <v>13.6899453248426</v>
+        <v>0.1733930869030597</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2198,7 +2198,7 @@
         <v>14.30057747071926</v>
       </c>
       <c r="C165">
-        <v>13.77815974321872</v>
+        <v>0.1728802003631158</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2209,7 +2209,7 @@
         <v>14.40054930713995</v>
       </c>
       <c r="C166">
-        <v>13.87063365719049</v>
+        <v>0.1726180389700098</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2220,7 +2220,7 @@
         <v>14.5005225171146</v>
       </c>
       <c r="C167">
-        <v>13.96316005378328</v>
+        <v>0.1718591597741046</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2231,7 +2231,7 @@
         <v>14.60049703365422</v>
       </c>
       <c r="C168">
-        <v>14.05404793095915</v>
+        <v>0.1720677493815556</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2242,7 +2242,7 @@
         <v>14.70047279303686</v>
       </c>
       <c r="C169">
-        <v>14.14432744701907</v>
+        <v>0.1726412648466004</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2253,7 +2253,7 @@
         <v>14.80044973464836</v>
       </c>
       <c r="C170">
-        <v>14.23487669236008</v>
+        <v>0.1735631700211432</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2264,7 +2264,7 @@
         <v>14.90042780083074</v>
       </c>
       <c r="C171">
-        <v>14.32354862349119</v>
+        <v>0.1731823624078601</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2275,7 +2275,7 @@
         <v>15.00040693673802</v>
       </c>
       <c r="C172">
-        <v>14.418654317642</v>
+        <v>0.1730486300528239</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2286,7 +2286,7 @@
         <v>15.10038709019912</v>
       </c>
       <c r="C173">
-        <v>14.51398707754502</v>
+        <v>0.172857897333578</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2297,7 +2297,7 @@
         <v>15.20036821158734</v>
       </c>
       <c r="C174">
-        <v>14.6090721149008</v>
+        <v>0.1729171060122482</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2308,7 +2308,7 @@
         <v>15.30035025369632</v>
       </c>
       <c r="C175">
-        <v>14.70390066621727</v>
+        <v>0.1724106206685961</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2319,7 +2319,7 @@
         <v>15.40033317162198</v>
       </c>
       <c r="C176">
-        <v>14.8026492726285</v>
+        <v>0.171991947879028</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2330,7 +2330,7 @@
         <v>15.50031692265023</v>
       </c>
       <c r="C177">
-        <v>14.9023016504586</v>
+        <v>0.172306207962095</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2341,7 +2341,7 @@
         <v>15.60030146615019</v>
       </c>
       <c r="C178">
-        <v>15.00046898997859</v>
+        <v>0.1729242364646934</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2352,7 +2352,7 @@
         <v>15.70028676347255</v>
       </c>
       <c r="C179">
-        <v>15.09904701224535</v>
+        <v>0.1728570738297795</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2363,7 +2363,7 @@
         <v>15.80027277785296</v>
       </c>
       <c r="C180">
-        <v>15.1915524726</v>
+        <v>0.1718300322839537</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2374,7 +2374,7 @@
         <v>15.90025947432009</v>
       </c>
       <c r="C181">
-        <v>15.28370119612768</v>
+        <v>0.1698870808622146</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2385,7 +2385,7 @@
         <v>16.00024681960817</v>
       </c>
       <c r="C182">
-        <v>15.3779970841807</v>
+        <v>0.1681683429465114</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2396,7 +2396,7 @@
         <v>16.10023478207384</v>
       </c>
       <c r="C183">
-        <v>15.4741543698923</v>
+        <v>0.1672949389280521</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2407,7 +2407,7 @@
         <v>16.20022333161698</v>
       </c>
       <c r="C184">
-        <v>15.57237097417673</v>
+        <v>0.1670049190421039</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2418,7 +2418,7 @@
         <v>16.3002124396055</v>
       </c>
       <c r="C185">
-        <v>15.67219651723555</v>
+        <v>0.1668973630783499</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2429,7 +2429,7 @@
         <v>16.40020207880368</v>
       </c>
       <c r="C186">
-        <v>15.76877794087872</v>
+        <v>0.1677568804074426</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2440,7 +2440,7 @@
         <v>16.50019222330412</v>
       </c>
       <c r="C187">
-        <v>15.87159741033224</v>
+        <v>0.1689595379883656</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2451,7 +2451,7 @@
         <v>16.60018284846296</v>
       </c>
       <c r="C188">
-        <v>15.97530710403532</v>
+        <v>0.1698208545414726</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2462,7 +2462,7 @@
         <v>16.70017393083819</v>
       </c>
       <c r="C189">
-        <v>16.08091116539057</v>
+        <v>0.1712280561498141</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2473,7 +2473,7 @@
         <v>16.80016544813111</v>
       </c>
       <c r="C190">
-        <v>16.19233342763203</v>
+        <v>0.173190551726343</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2484,7 +2484,7 @@
         <v>16.90015737913055</v>
       </c>
       <c r="C191">
-        <v>16.29949528146077</v>
+        <v>0.1750680038684923</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2495,7 +2495,7 @@
         <v>17.00014970365978</v>
       </c>
       <c r="C192">
-        <v>16.41267030290956</v>
+        <v>0.1764207157913076</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2506,7 +2506,7 @@
         <v>17.10014240252614</v>
       </c>
       <c r="C193">
-        <v>16.52146049382485</v>
+        <v>0.1771212881024317</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2517,7 +2517,7 @@
         <v>17.20013545747299</v>
       </c>
       <c r="C194">
-        <v>16.63081172738521</v>
+        <v>0.177631498495938</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2528,7 +2528,7 @@
         <v>17.30012885113407</v>
       </c>
       <c r="C195">
-        <v>16.73392997978733</v>
+        <v>0.1777693734938198</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2539,7 +2539,7 @@
         <v>17.40012256699011</v>
       </c>
       <c r="C196">
-        <v>16.83906093149868</v>
+        <v>0.1778800365771651</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2550,7 +2550,7 @@
         <v>17.50011658932746</v>
       </c>
       <c r="C197">
-        <v>16.94165097123996</v>
+        <v>0.1782048631330038</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -2561,7 +2561,7 @@
         <v>17.60011090319886</v>
       </c>
       <c r="C198">
-        <v>17.04790973144757</v>
+        <v>0.1792295752563274</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -2572,7 +2572,7 @@
         <v>17.70010549438603</v>
       </c>
       <c r="C199">
-        <v>17.15589426932403</v>
+        <v>0.1801542134609537</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -2583,7 +2583,7 @@
         <v>17.80010034936411</v>
       </c>
       <c r="C200">
-        <v>17.2646745886772</v>
+        <v>0.1789090732506517</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2594,7 +2594,7 @@
         <v>17.90009545526788</v>
       </c>
       <c r="C201">
-        <v>17.37288175943135</v>
+        <v>0.1775143172406193</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -2605,7 +2605,7 @@
         <v>18.00009079985952</v>
       </c>
       <c r="C202">
-        <v>17.48319434379392</v>
+        <v>0.1766690856741217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Names and Directory
Structures and saving methods were changed for organization
</commit_message>
<xml_diff>
--- a/MSD Results/msd_100.xlsx
+++ b/MSD Results/msd_100.xlsx
@@ -427,7 +427,7 @@
         <v>0.009674836071919213</v>
       </c>
       <c r="C4">
-        <v>0.009753288441728696</v>
+        <v>0.009766928276264165</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -438,7 +438,7 @@
         <v>0.02141595285011544</v>
       </c>
       <c r="C5">
-        <v>0.02157659858511547</v>
+        <v>0.02156083928521075</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -449,7 +449,7 @@
         <v>0.03746150615596378</v>
       </c>
       <c r="C6">
-        <v>0.0377849253088377</v>
+        <v>0.03768389350446941</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -460,7 +460,7 @@
         <v>0.05760156614280998</v>
       </c>
       <c r="C7">
-        <v>0.05812028643739596</v>
+        <v>0.05793087251842101</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -471,7 +471,7 @@
         <v>0.08163644136343606</v>
       </c>
       <c r="C8">
-        <v>0.08231289993266075</v>
+        <v>0.08211674818633509</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -482,7 +482,7 @@
         <v>0.1093761794374268</v>
       </c>
       <c r="C9">
-        <v>0.1101107626374209</v>
+        <v>0.1100196358716836</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -493,7 +493,7 @@
         <v>0.1406400920712789</v>
       </c>
       <c r="C10">
-        <v>0.1413572371700808</v>
+        <v>0.1413907157287204</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -504,7 +504,7 @@
         <v>0.1752563032435468</v>
       </c>
       <c r="C11">
-        <v>0.1758132597114231</v>
+        <v>0.1759662852151182</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -515,7 +515,7 @@
         <v>0.2130613194252668</v>
       </c>
       <c r="C12">
-        <v>0.213531362051066</v>
+        <v>0.2135316288410345</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -526,7 +526,7 @@
         <v>0.2538996207609734</v>
       </c>
       <c r="C13">
-        <v>0.2542871859734577</v>
+        <v>0.2539119324223771</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -537,7 +537,7 @@
         <v>0.2976232721880532</v>
       </c>
       <c r="C14">
-        <v>0.2980824994059056</v>
+        <v>0.2973456529191318</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -548,7 +548,7 @@
         <v>0.3440915535220324</v>
       </c>
       <c r="C15">
-        <v>0.3441330044857458</v>
+        <v>0.343301632711253</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -559,7 +559,7 @@
         <v>0.3931706075828192</v>
       </c>
       <c r="C16">
-        <v>0.3932446638739931</v>
+        <v>0.3917782546298345</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -570,7 +570,7 @@
         <v>0.4447331054820296</v>
       </c>
       <c r="C17">
-        <v>0.4449773431519968</v>
+        <v>0.4431988432875831</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -581,7 +581,7 @@
         <v>0.4986579282344432</v>
       </c>
       <c r="C18">
-        <v>0.4987681814223643</v>
+        <v>0.4971398688432354</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -592,7 +592,7 @@
         <v>0.5548298638974534</v>
       </c>
       <c r="C19">
-        <v>0.5550933730433075</v>
+        <v>0.5537000682763866</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -603,7 +603,7 @@
         <v>0.6131393194811983</v>
       </c>
       <c r="C20">
-        <v>0.6139976142488555</v>
+        <v>0.6122808058000074</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -614,7 +614,7 @@
         <v>0.6734820469090024</v>
       </c>
       <c r="C21">
-        <v>0.6745541167018773</v>
+        <v>0.6728804180902944</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -625,7 +625,7 @@
         <v>0.7357588823428847</v>
       </c>
       <c r="C22">
-        <v>0.7374691439830344</v>
+        <v>0.7343504337700244</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -636,7 +636,7 @@
         <v>0.7998754982223106</v>
       </c>
       <c r="C23">
-        <v>0.8017998987415691</v>
+        <v>0.7982936451717921</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -647,7 +647,7 @@
         <v>0.8657421673961592</v>
       </c>
       <c r="C24">
-        <v>0.8679264410609109</v>
+        <v>0.864130012066739</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -658,7 +658,7 @@
         <v>0.9332735387581064</v>
       </c>
       <c r="C25">
-        <v>0.9366483194812001</v>
+        <v>0.9310223292982482</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -669,7 +669,7 @@
         <v>1.002388423824404</v>
       </c>
       <c r="C26">
-        <v>1.006951038414591</v>
+        <v>1.000176066246037</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -680,7 +680,7 @@
         <v>1.07300959372038</v>
       </c>
       <c r="C27">
-        <v>1.079094312534609</v>
+        <v>1.069881444109924</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -691,7 +691,7 @@
         <v>1.145063586068025</v>
       </c>
       <c r="C28">
-        <v>1.152540731233806</v>
+        <v>1.140771356907071</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -702,7 +702,7 @@
         <v>1.218480521291783</v>
       </c>
       <c r="C29">
-        <v>1.226309393504759</v>
+        <v>1.21348372823346</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -713,7 +713,7 @@
         <v>1.293193927883213</v>
       </c>
       <c r="C30">
-        <v>1.30142877373184</v>
+        <v>1.286911438463979</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -724,7 +724,7 @@
         <v>1.369140576187596</v>
       </c>
       <c r="C31">
-        <v>1.377087506742659</v>
+        <v>1.362170694584545</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -735,7 +735,7 @@
         <v>1.44626032029686</v>
       </c>
       <c r="C32">
-        <v>1.451951361756234</v>
+        <v>1.43818385021918</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -746,7 +746,7 @@
         <v>1.524495947653486</v>
       </c>
       <c r="C33">
-        <v>1.528488935384992</v>
+        <v>1.515799656775276</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -757,7 +757,7 @@
         <v>1.603793035989311</v>
       </c>
       <c r="C34">
-        <v>1.605886033647769</v>
+        <v>1.595274869848191</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -768,7 +768,7 @@
         <v>1.684099817241508</v>
       </c>
       <c r="C35">
-        <v>1.684791714549768</v>
+        <v>1.677115880604857</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -779,7 +779,7 @@
         <v>1.76536704810547</v>
       </c>
       <c r="C36">
-        <v>1.766427128453978</v>
+        <v>1.759145847139342</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -790,7 +790,7 @@
         <v>1.84754788690089</v>
       </c>
       <c r="C37">
-        <v>1.850068774031568</v>
+        <v>1.84197027695373</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -801,7 +801,7 @@
         <v>1.930597776443173</v>
       </c>
       <c r="C38">
-        <v>1.934943355299791</v>
+        <v>1.924590493193331</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -812,7 +812,7 @@
         <v>2.014474332627255</v>
       </c>
       <c r="C39">
-        <v>2.020400043623249</v>
+        <v>2.008114440913517</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -823,7 +823,7 @@
         <v>2.09913723844527</v>
       </c>
       <c r="C40">
-        <v>2.106714956667689</v>
+        <v>2.093482771941306</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -834,7 +834,7 @@
         <v>2.184548143173028</v>
       </c>
       <c r="C41">
-        <v>2.194006196836227</v>
+        <v>2.181104635333345</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -845,7 +845,7 @@
         <v>2.270670566473226</v>
       </c>
       <c r="C42">
-        <v>2.281261571946917</v>
+        <v>2.268919388456272</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -856,7 +856,7 @@
         <v>2.357469807175609</v>
       </c>
       <c r="C43">
-        <v>2.368985090193066</v>
+        <v>2.358463849815404</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -867,7 +867,7 @@
         <v>2.444912856505964</v>
       </c>
       <c r="C44">
-        <v>2.456820567529328</v>
+        <v>2.448541345077498</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -878,7 +878,7 @@
         <v>2.532968315546993</v>
       </c>
       <c r="C45">
-        <v>2.545835954395754</v>
+        <v>2.538289984065774</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -889,7 +889,7 @@
         <v>2.621606316724668</v>
       </c>
       <c r="C46">
-        <v>2.634234613249705</v>
+        <v>2.629027880529704</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -900,7 +900,7 @@
         <v>2.710798449123729</v>
       </c>
       <c r="C47">
-        <v>2.725825304919247</v>
+        <v>2.719752913221949</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -911,7 +911,7 @@
         <v>2.800517687445608</v>
       </c>
       <c r="C48">
-        <v>2.818972240099197</v>
+        <v>2.811270678689108</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -922,7 +922,7 @@
         <v>2.8907383244311</v>
       </c>
       <c r="C49">
-        <v>2.913025734881148</v>
+        <v>2.903231025592738</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -933,7 +933,7 @@
         <v>2.981435906578826</v>
       </c>
       <c r="C50">
-        <v>3.007044382615518</v>
+        <v>2.995958196681791</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -944,7 +944,7 @@
         <v>3.072587172998741</v>
       </c>
       <c r="C51">
-        <v>3.101783469974173</v>
+        <v>3.088603669196094</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -955,7 +955,7 @@
         <v>3.164169997247797</v>
       </c>
       <c r="C52">
-        <v>3.196765909754238</v>
+        <v>3.181193091226759</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -966,7 +966,7 @@
         <v>3.256163332002306</v>
       </c>
       <c r="C53">
-        <v>3.292417848555297</v>
+        <v>3.274148995459111</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -977,7 +977,7 @@
         <v>3.348547156428668</v>
       </c>
       <c r="C54">
-        <v>3.386997148009073</v>
+        <v>3.368210784214019</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -988,7 +988,7 @@
         <v>3.44130242612086</v>
       </c>
       <c r="C55">
-        <v>3.484233884631472</v>
+        <v>3.461719621408712</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -999,7 +999,7 @@
         <v>3.5344110254795</v>
       </c>
       <c r="C56">
-        <v>3.581537370759428</v>
+        <v>3.555979297342192</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1010,7 +1010,7 @@
         <v>3.627855722413415</v>
       </c>
       <c r="C57">
-        <v>3.675650844039735</v>
+        <v>3.648939620356668</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1021,7 +1021,7 @@
         <v>3.721620125250436</v>
       </c>
       <c r="C58">
-        <v>3.770374924849635</v>
+        <v>3.743141749368196</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1032,7 +1032,7 @@
         <v>3.815688641749677</v>
       </c>
       <c r="C59">
-        <v>3.864745806903871</v>
+        <v>3.838665717662304</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1043,7 +1043,7 @@
         <v>3.910046440112815</v>
       </c>
       <c r="C60">
-        <v>3.961427760206349</v>
+        <v>3.932494679593262</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1054,7 +1054,7 @@
         <v>4.004679411896865</v>
       </c>
       <c r="C61">
-        <v>4.060040129570856</v>
+        <v>4.024561117870975</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1065,7 +1065,7 @@
         <v>4.099574136735728</v>
       </c>
       <c r="C62">
-        <v>4.157540562788473</v>
+        <v>4.117808827899569</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1076,7 +1076,7 @@
         <v>4.194717848782282</v>
       </c>
       <c r="C63">
-        <v>4.253690681866249</v>
+        <v>4.208724950245021</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1087,7 +1087,7 @@
         <v>4.290098404787115</v>
       </c>
       <c r="C64">
-        <v>4.34976252190444</v>
+        <v>4.301433155321211</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1098,7 +1098,7 @@
         <v>4.385704253734081</v>
       </c>
       <c r="C65">
-        <v>4.445567513285054</v>
+        <v>4.395755572004175</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1109,7 +1109,7 @@
         <v>4.481524407956733</v>
       </c>
       <c r="C66">
-        <v>4.540033283819307</v>
+        <v>4.488407007259687</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1120,7 +1120,7 @@
         <v>4.577548415663444</v>
       </c>
       <c r="C67">
-        <v>4.636305740418603</v>
+        <v>4.579221823869865</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1131,7 +1131,7 @@
         <v>4.67376633480248</v>
       </c>
       <c r="C68">
-        <v>4.733326002505752</v>
+        <v>4.671802879197249</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1142,7 +1142,7 @@
         <v>4.77016870820169</v>
       </c>
       <c r="C69">
-        <v>4.829281572553685</v>
+        <v>4.767169018631933</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1153,7 +1153,7 @@
         <v>4.866746539920653</v>
       </c>
       <c r="C70">
-        <v>4.92808018648923</v>
+        <v>4.861708928410478</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1164,7 +1164,7 @@
         <v>4.963491272756136</v>
       </c>
       <c r="C71">
-        <v>5.029435177514951</v>
+        <v>4.956754837452218</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1175,7 +1175,7 @@
         <v>5.060394766844637</v>
       </c>
       <c r="C72">
-        <v>5.132984571960407</v>
+        <v>5.052683243365809</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1186,7 +1186,7 @@
         <v>5.157449279308479</v>
       </c>
       <c r="C73">
-        <v>5.233743657854486</v>
+        <v>5.146942548177481</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1197,7 +1197,7 @@
         <v>5.254647444894585</v>
       </c>
       <c r="C74">
-        <v>5.334584048639293</v>
+        <v>5.241017865701242</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1208,7 +1208,7 @@
         <v>5.351982257557512</v>
       </c>
       <c r="C75">
-        <v>5.434030633064582</v>
+        <v>5.338009662340804</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1219,7 +1219,7 @@
         <v>5.44944705294068</v>
       </c>
       <c r="C76">
-        <v>5.534610045979209</v>
+        <v>5.434880067029571</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1230,7 +1230,7 @@
         <v>5.547035491712018</v>
       </c>
       <c r="C77">
-        <v>5.636414551632722</v>
+        <v>5.530137835552329</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1241,7 +1241,7 @@
         <v>5.644741543712332</v>
       </c>
       <c r="C78">
-        <v>5.737600592654746</v>
+        <v>5.625037240060605</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1252,7 +1252,7 @@
         <v>5.742559472876755</v>
       </c>
       <c r="C79">
-        <v>5.838238762418049</v>
+        <v>5.720688333770771</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1263,7 +1263,7 @@
         <v>5.84048382289161</v>
       </c>
       <c r="C80">
-        <v>5.939462332274943</v>
+        <v>5.819383002566001</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1274,7 +1274,7 @@
         <v>5.938509403550774</v>
       </c>
       <c r="C81">
-        <v>6.040362256539602</v>
+        <v>5.915852666985556</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1285,7 +1285,7 @@
         <v>6.036631277777468</v>
       </c>
       <c r="C82">
-        <v>6.142296672777496</v>
+        <v>6.012487754312793</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1296,7 +1296,7 @@
         <v>6.134844749278987</v>
       </c>
       <c r="C83">
-        <v>6.242743397262635</v>
+        <v>6.108698404793738</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1307,7 +1307,7 @@
         <v>6.233145350803523</v>
       </c>
       <c r="C84">
-        <v>6.343388926739173</v>
+        <v>6.202834244494725</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1318,7 +1318,7 @@
         <v>6.33152883296971</v>
       </c>
       <c r="C85">
-        <v>6.442820551434512</v>
+        <v>6.297354310099582</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1329,7 +1329,7 @@
         <v>6.429991153640955</v>
       </c>
       <c r="C86">
-        <v>6.54199806931549</v>
+        <v>6.394385161422254</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1340,7 +1340,7 @@
         <v>6.528528467817999</v>
       </c>
       <c r="C87">
-        <v>6.642444631282885</v>
+        <v>6.488578142800312</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1351,7 +1351,7 @@
         <v>6.627137118024402</v>
       </c>
       <c r="C88">
-        <v>6.742172926395744</v>
+        <v>6.579678569901363</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1362,7 +1362,7 @@
         <v>6.72581362516096</v>
       </c>
       <c r="C89">
-        <v>6.843337769150001</v>
+        <v>6.669389456221282</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1373,7 +1373,7 @@
         <v>6.824554679806138</v>
       </c>
       <c r="C90">
-        <v>6.942168243712032</v>
+        <v>6.760815486724486</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1384,7 +1384,7 @@
         <v>6.923357133940792</v>
       </c>
       <c r="C91">
-        <v>7.038642118987839</v>
+        <v>6.852005244680887</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1395,7 +1395,7 @@
         <v>7.022217993076485</v>
       </c>
       <c r="C92">
-        <v>7.135013694498836</v>
+        <v>6.943584247241769</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1406,7 +1406,7 @@
         <v>7.121134408767706</v>
       </c>
       <c r="C93">
-        <v>7.233128501390492</v>
+        <v>7.034341550429226</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1417,7 +1417,7 @@
         <v>7.220103671489268</v>
       </c>
       <c r="C94">
-        <v>7.332246337792009</v>
+        <v>7.122763647494867</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1428,7 +1428,7 @@
         <v>7.319123203861087</v>
       </c>
       <c r="C95">
-        <v>7.43389864162849</v>
+        <v>7.211731110977082</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1439,7 +1439,7 @@
         <v>7.418190554203392</v>
       </c>
       <c r="C96">
-        <v>7.536982371312396</v>
+        <v>7.299280065161661</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1450,7 +1450,7 @@
         <v>7.517303390406241</v>
       </c>
       <c r="C97">
-        <v>7.640948627536591</v>
+        <v>7.387109944488856</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1461,7 +1461,7 @@
         <v>7.616459494098041</v>
       </c>
       <c r="C98">
-        <v>7.746357369998607</v>
+        <v>7.472961584494465</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1472,7 +1472,7 @@
         <v>7.715656755098452</v>
       </c>
       <c r="C99">
-        <v>7.853735898449598</v>
+        <v>7.558220941875952</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1483,7 +1483,7 @@
         <v>7.81489316614185</v>
       </c>
       <c r="C100">
-        <v>7.959548978743338</v>
+        <v>7.64199171280158</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1494,7 +1494,7 @@
         <v>7.914166817858105</v>
       </c>
       <c r="C101">
-        <v>8.06647836357952</v>
+        <v>7.727326328020477</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1505,7 +1505,7 @@
         <v>8.013475893998171</v>
       </c>
       <c r="C102">
-        <v>8.172781888151736</v>
+        <v>7.813545461685887</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1516,7 +1516,7 @@
         <v>8.112818666892514</v>
       </c>
       <c r="C103">
-        <v>8.280765608787977</v>
+        <v>7.900877104352147</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1527,7 +1527,7 @@
         <v>8.212193493131032</v>
       </c>
       <c r="C104">
-        <v>8.387800301224257</v>
+        <v>7.989663340852015</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1538,7 +1538,7 @@
         <v>8.311598809453685</v>
       </c>
       <c r="C105">
-        <v>8.493239859616766</v>
+        <v>8.082023733375244</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1549,7 +1549,7 @@
         <v>8.411033128841522</v>
       </c>
       <c r="C106">
-        <v>8.598519078563768</v>
+        <v>8.175969354564662</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1560,7 +1560,7 @@
         <v>8.510495036798362</v>
       </c>
       <c r="C107">
-        <v>8.700628490773145</v>
+        <v>8.268061791159271</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1571,7 +1571,7 @@
         <v>8.609983187813821</v>
       </c>
       <c r="C108">
-        <v>8.802098570257716</v>
+        <v>8.363709643440774</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1582,7 +1582,7 @@
         <v>8.709496301998824</v>
       </c>
       <c r="C109">
-        <v>8.906071375614323</v>
+        <v>8.459151285024179</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1593,7 +1593,7 @@
         <v>8.809033161885226</v>
       </c>
       <c r="C110">
-        <v>9.008814499444167</v>
+        <v>8.55250464498797</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1604,7 +1604,7 @@
         <v>8.908592609381506</v>
       </c>
       <c r="C111">
-        <v>9.109550416528609</v>
+        <v>8.645657190166572</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1615,7 +1615,7 @@
         <v>9.008173542876929</v>
       </c>
       <c r="C112">
-        <v>9.211282297120452</v>
+        <v>8.741644233342114</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1626,7 +1626,7 @@
         <v>9.107774914486953</v>
       </c>
       <c r="C113">
-        <v>9.311879187490629</v>
+        <v>8.836654362834368</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -1637,7 +1637,7 @@
         <v>9.207395727432967</v>
       </c>
       <c r="C114">
-        <v>9.416582383104572</v>
+        <v>8.931199023117294</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1648,7 +1648,7 @@
         <v>9.307035033549825</v>
       </c>
       <c r="C115">
-        <v>9.521891850989215</v>
+        <v>9.024501552602111</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1659,7 +1659,7 @@
         <v>9.406691930914944</v>
       </c>
       <c r="C116">
-        <v>9.627382337926939</v>
+        <v>9.118876695039441</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1670,7 +1670,7 @@
         <v>9.50636556159302</v>
       </c>
       <c r="C117">
-        <v>9.732817898636782</v>
+        <v>9.213171743907242</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1681,7 +1681,7 @@
         <v>9.606055109490754</v>
       </c>
       <c r="C118">
-        <v>9.838889890139484</v>
+        <v>9.304765471661725</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1692,7 +1692,7 @@
         <v>9.705759798316178</v>
       </c>
       <c r="C119">
-        <v>9.943144134795773</v>
+        <v>9.398580788113756</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1703,7 +1703,7 @@
         <v>9.805478889637538</v>
       </c>
       <c r="C120">
-        <v>10.04691939994323</v>
+        <v>9.491363616619351</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1714,7 +1714,7 @@
         <v>9.905211681036818</v>
       </c>
       <c r="C121">
-        <v>10.14923014534803</v>
+        <v>9.583222948680124</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1725,7 +1725,7 @@
         <v>10.00495750435333</v>
       </c>
       <c r="C122">
-        <v>10.24978726812698</v>
+        <v>9.673925468278078</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1736,7 +1736,7 @@
         <v>10.10471572401298</v>
       </c>
       <c r="C123">
-        <v>10.3543031051886</v>
+        <v>9.763477625451047</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1747,7 +1747,7 @@
         <v>10.20448573543897</v>
       </c>
       <c r="C124">
-        <v>10.4587894662314</v>
+        <v>9.852438853478587</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1758,7 +1758,7 @@
         <v>10.30426696354008</v>
       </c>
       <c r="C125">
-        <v>10.5621545016005</v>
+        <v>9.943005646028384</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1769,7 +1769,7 @@
         <v>10.40405886127259</v>
       </c>
       <c r="C126">
-        <v>10.66402407495465</v>
+        <v>10.02795287859986</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1780,7 +1780,7 @@
         <v>10.50386090827246</v>
       </c>
       <c r="C127">
-        <v>10.76247371725452</v>
+        <v>10.11750849323839</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1791,7 +1791,7 @@
         <v>10.60367260955406</v>
       </c>
       <c r="C128">
-        <v>10.85918810972141</v>
+        <v>10.20696737665774</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1802,7 +1802,7 @@
         <v>10.70349349427252</v>
       </c>
       <c r="C129">
-        <v>10.9536872385345</v>
+        <v>10.3013722155928</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1813,7 +1813,7 @@
         <v>10.80332311454635</v>
       </c>
       <c r="C130">
-        <v>11.04609334826881</v>
+        <v>10.39733642429015</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1824,7 +1824,7 @@
         <v>10.90316104433747</v>
       </c>
       <c r="C131">
-        <v>11.13724717078817</v>
+        <v>10.49611502842655</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1835,7 +1835,7 @@
         <v>11.00300687838596</v>
       </c>
       <c r="C132">
-        <v>11.22607104465442</v>
+        <v>10.59702391712197</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1846,7 +1846,7 @@
         <v>11.10286023119662</v>
       </c>
       <c r="C133">
-        <v>11.31715298187858</v>
+        <v>10.69879500701096</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1857,7 +1857,7 @@
         <v>11.2027207360751</v>
       </c>
       <c r="C134">
-        <v>11.40786227100048</v>
+        <v>10.80214591397073</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1868,7 +1868,7 @@
         <v>11.30258804421093</v>
       </c>
       <c r="C135">
-        <v>11.49662622030412</v>
+        <v>10.90575053299088</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1879,7 +1879,7 @@
         <v>11.40246182380535</v>
       </c>
       <c r="C136">
-        <v>11.58696438994979</v>
+        <v>11.00600041588144</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1890,7 +1890,7 @@
         <v>11.50234175924158</v>
       </c>
       <c r="C137">
-        <v>11.68065592770288</v>
+        <v>11.10405873561306</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1901,7 +1901,7 @@
         <v>11.60222755029569</v>
       </c>
       <c r="C138">
-        <v>11.77598414573585</v>
+        <v>11.20267411895002</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -1912,7 +1912,7 @@
         <v>11.70211891138582</v>
       </c>
       <c r="C139">
-        <v>11.87217648173922</v>
+        <v>11.2984956755699</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -1923,7 +1923,7 @@
         <v>11.8020155708581</v>
       </c>
       <c r="C140">
-        <v>11.96628536354504</v>
+        <v>11.39288210652145</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1934,7 +1934,7 @@
         <v>11.90191727030739</v>
       </c>
       <c r="C141">
-        <v>12.05920621382399</v>
+        <v>11.48717716540073</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -1945,7 +1945,7 @@
         <v>12.00182376393111</v>
       </c>
       <c r="C142">
-        <v>12.15212218231508</v>
+        <v>11.58149565068853</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -1956,7 +1956,7 @@
         <v>12.10173481791461</v>
       </c>
       <c r="C143">
-        <v>12.2446912030152</v>
+        <v>11.67324617846016</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -1967,7 +1967,7 @@
         <v>12.20165020984653</v>
       </c>
       <c r="C144">
-        <v>12.33719903430569</v>
+        <v>11.76809160584478</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -1978,7 +1978,7 @@
         <v>12.30156972816262</v>
       </c>
       <c r="C145">
-        <v>12.4326299533795</v>
+        <v>11.86394489766182</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -1989,7 +1989,7 @@
         <v>12.40149317161675</v>
       </c>
       <c r="C146">
-        <v>12.52529550603547</v>
+        <v>11.96190096850571</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2000,7 +2000,7 @@
         <v>12.50142034877769</v>
       </c>
       <c r="C147">
-        <v>12.61982027458507</v>
+        <v>12.05871364487362</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2011,7 +2011,7 @@
         <v>12.60135107755039</v>
       </c>
       <c r="C148">
-        <v>12.71395120071835</v>
+        <v>12.15657851317827</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2022,7 +2022,7 @@
         <v>12.70128518472071</v>
       </c>
       <c r="C149">
-        <v>12.80767606627469</v>
+        <v>12.25113801976408</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2033,7 +2033,7 @@
         <v>12.80122250552226</v>
       </c>
       <c r="C150">
-        <v>12.90350786082815</v>
+        <v>12.34322529211937</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2044,7 +2044,7 @@
         <v>12.90116288322439</v>
       </c>
       <c r="C151">
-        <v>13.0007747065924</v>
+        <v>12.43043409176714</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2055,7 +2055,7 @@
         <v>13.0011061687403</v>
       </c>
       <c r="C152">
-        <v>13.10228358961356</v>
+        <v>12.51756517225301</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2066,7 +2066,7 @@
         <v>13.10105222025423</v>
       </c>
       <c r="C153">
-        <v>13.20606072448316</v>
+        <v>12.60355781575264</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2077,7 +2077,7 @@
         <v>13.20100090286688</v>
       </c>
       <c r="C154">
-        <v>13.31153567878317</v>
+        <v>12.68910508564745</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2088,7 +2088,7 @@
         <v>13.30095208825804</v>
       </c>
       <c r="C155">
-        <v>13.4177142191087</v>
+        <v>12.77950347318619</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2099,7 +2099,7 @@
         <v>13.40090565436577</v>
       </c>
       <c r="C156">
-        <v>13.52678633493841</v>
+        <v>12.87032112335066</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2110,7 +2110,7 @@
         <v>13.50086148508115</v>
       </c>
       <c r="C157">
-        <v>13.63442590852943</v>
+        <v>12.96324352276563</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2121,7 +2121,7 @@
         <v>13.60081946995796</v>
       </c>
       <c r="C158">
-        <v>13.73869497115676</v>
+        <v>13.05085469146212</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2132,7 +2132,7 @@
         <v>13.70077950393651</v>
       </c>
       <c r="C159">
-        <v>13.84401648078742</v>
+        <v>13.13854776065747</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2143,7 +2143,7 @@
         <v>13.80074148708092</v>
       </c>
       <c r="C160">
-        <v>13.95167232267918</v>
+        <v>13.22536211229055</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2154,7 +2154,7 @@
         <v>13.90070532432926</v>
       </c>
       <c r="C161">
-        <v>14.0612866801442</v>
+        <v>13.31097588638839</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2165,7 +2165,7 @@
         <v>14.0006709252558</v>
       </c>
       <c r="C162">
-        <v>14.17034082270536</v>
+        <v>13.39691901929483</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2176,7 +2176,7 @@
         <v>14.10063820384496</v>
       </c>
       <c r="C163">
-        <v>14.27888605225901</v>
+        <v>13.48285162466797</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2187,7 +2187,7 @@
         <v>14.20060707827616</v>
       </c>
       <c r="C164">
-        <v>14.39130526706446</v>
+        <v>13.56731330434999</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2198,7 +2198,7 @@
         <v>14.30057747071926</v>
       </c>
       <c r="C165">
-        <v>14.50271241494064</v>
+        <v>13.65458681000866</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2209,7 +2209,7 @@
         <v>14.40054930713995</v>
       </c>
       <c r="C166">
-        <v>14.61067202390536</v>
+        <v>13.73990182786301</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2220,7 +2220,7 @@
         <v>14.5005225171146</v>
       </c>
       <c r="C167">
-        <v>14.72031815349435</v>
+        <v>13.82891538799531</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2231,7 +2231,7 @@
         <v>14.60049703365422</v>
       </c>
       <c r="C168">
-        <v>14.82761596286206</v>
+        <v>13.91494125557686</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2242,7 +2242,7 @@
         <v>14.70047279303686</v>
       </c>
       <c r="C169">
-        <v>14.93986475648772</v>
+        <v>14.00058640158587</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2253,7 +2253,7 @@
         <v>14.80044973464836</v>
       </c>
       <c r="C170">
-        <v>15.05219716469028</v>
+        <v>14.08806284497787</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2264,7 +2264,7 @@
         <v>14.90042780083074</v>
       </c>
       <c r="C171">
-        <v>15.16687475470046</v>
+        <v>14.17807687084446</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2275,7 +2275,7 @@
         <v>15.00040693673802</v>
       </c>
       <c r="C172">
-        <v>15.27940854531719</v>
+        <v>14.2679642008113</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2286,7 +2286,7 @@
         <v>15.10038709019912</v>
       </c>
       <c r="C173">
-        <v>15.39170306395946</v>
+        <v>14.35785687957468</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2297,7 +2297,7 @@
         <v>15.20036821158734</v>
       </c>
       <c r="C174">
-        <v>15.50280662600399</v>
+        <v>14.44955472965438</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2308,7 +2308,7 @@
         <v>15.30035025369632</v>
       </c>
       <c r="C175">
-        <v>15.61120614549797</v>
+        <v>14.54354972690854</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2319,7 +2319,7 @@
         <v>15.40033317162198</v>
       </c>
       <c r="C176">
-        <v>15.72034013011253</v>
+        <v>14.64088877572349</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2330,7 +2330,7 @@
         <v>15.50031692265023</v>
       </c>
       <c r="C177">
-        <v>15.83154420703538</v>
+        <v>14.74130301920446</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2341,7 +2341,7 @@
         <v>15.60030146615019</v>
       </c>
       <c r="C178">
-        <v>15.9382025411333</v>
+        <v>14.84174189483419</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2352,7 +2352,7 @@
         <v>15.70028676347255</v>
       </c>
       <c r="C179">
-        <v>16.04509280920497</v>
+        <v>14.94210159480829</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2363,7 +2363,7 @@
         <v>15.80027277785296</v>
       </c>
       <c r="C180">
-        <v>16.15036396659199</v>
+        <v>15.0425224073348</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2374,7 +2374,7 @@
         <v>15.90025947432009</v>
       </c>
       <c r="C181">
-        <v>16.25385104247145</v>
+        <v>15.14475285297704</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2385,7 +2385,7 @@
         <v>16.00024681960817</v>
       </c>
       <c r="C182">
-        <v>16.35906021871976</v>
+        <v>15.24934689628938</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2396,7 +2396,7 @@
         <v>16.10023478207384</v>
       </c>
       <c r="C183">
-        <v>16.46629395489081</v>
+        <v>15.35457087821087</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2407,7 +2407,7 @@
         <v>16.20022333161698</v>
       </c>
       <c r="C184">
-        <v>16.57216785012297</v>
+        <v>15.45830586871507</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2418,7 +2418,7 @@
         <v>16.3002124396055</v>
       </c>
       <c r="C185">
-        <v>16.67968808668192</v>
+        <v>15.56005149572838</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2429,7 +2429,7 @@
         <v>16.40020207880368</v>
       </c>
       <c r="C186">
-        <v>16.78658714979962</v>
+        <v>15.66293786430422</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2440,7 +2440,7 @@
         <v>16.50019222330412</v>
       </c>
       <c r="C187">
-        <v>16.89309141839559</v>
+        <v>15.76546138198191</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2451,7 +2451,7 @@
         <v>16.60018284846296</v>
       </c>
       <c r="C188">
-        <v>16.99491645328873</v>
+        <v>15.86938494292997</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2462,7 +2462,7 @@
         <v>16.70017393083819</v>
       </c>
       <c r="C189">
-        <v>17.08917301996411</v>
+        <v>15.97443903842094</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2473,7 +2473,7 @@
         <v>16.80016544813111</v>
       </c>
       <c r="C190">
-        <v>17.18793115066483</v>
+        <v>16.07855422483054</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2484,7 +2484,7 @@
         <v>16.90015737913055</v>
       </c>
       <c r="C191">
-        <v>17.28993101523923</v>
+        <v>16.18456968737577</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2495,7 +2495,7 @@
         <v>17.00014970365978</v>
       </c>
       <c r="C192">
-        <v>17.39431206967919</v>
+        <v>16.2845129709932</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2506,7 +2506,7 @@
         <v>17.10014240252614</v>
       </c>
       <c r="C193">
-        <v>17.49866195483611</v>
+        <v>16.38193792587768</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2517,7 +2517,7 @@
         <v>17.20013545747299</v>
       </c>
       <c r="C194">
-        <v>17.60713391304612</v>
+        <v>16.47834618310264</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2528,7 +2528,7 @@
         <v>17.30012885113407</v>
       </c>
       <c r="C195">
-        <v>17.71097466710536</v>
+        <v>16.57680089591404</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2539,7 +2539,7 @@
         <v>17.40012256699011</v>
       </c>
       <c r="C196">
-        <v>17.81341581999005</v>
+        <v>16.67592593033145</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2550,7 +2550,7 @@
         <v>17.50011658932746</v>
       </c>
       <c r="C197">
-        <v>17.91603479541428</v>
+        <v>16.77511565391696</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -2561,7 +2561,7 @@
         <v>17.60011090319886</v>
       </c>
       <c r="C198">
-        <v>18.02199227282831</v>
+        <v>16.8719277457567</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -2572,7 +2572,7 @@
         <v>17.70010549438603</v>
       </c>
       <c r="C199">
-        <v>18.13147382115434</v>
+        <v>16.97346938778329</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -2583,7 +2583,7 @@
         <v>17.80010034936411</v>
       </c>
       <c r="C200">
-        <v>18.23930657354244</v>
+        <v>17.07493884558764</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2594,7 +2594,7 @@
         <v>17.90009545526788</v>
       </c>
       <c r="C201">
-        <v>18.34889960256974</v>
+        <v>17.17398187986439</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -2605,7 +2605,7 @@
         <v>18.00009079985952</v>
       </c>
       <c r="C202">
-        <v>18.46231887340213</v>
+        <v>17.27137236196538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>